<commit_message>
Update effort_commitment - full times.xlsx
</commit_message>
<xml_diff>
--- a/documentation/budget/effort_commitment - full times.xlsx
+++ b/documentation/budget/effort_commitment - full times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Documents\Year 2\Professional Development\Phishing-Email-Button\documentation\budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CD42D6-D93F-416A-84ED-09187881E388}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B3DFDA-A3AA-49AE-B66A-C97586883721}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{38A891E2-6AF6-49EC-89C7-71415C5CC21F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="48">
   <si>
     <t>Starting Criteria</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Neil Fredrickson (Tech Lead)</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Christmas</t>
   </si>
 </sst>
 </file>
@@ -198,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +232,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
@@ -409,6 +427,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A4048D-0B48-4A1A-A71C-86F5C3BC7E01}">
   <dimension ref="B1:AG47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="L12" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1437,6 +1457,18 @@
       </c>
       <c r="C19" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="L19" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O19" s="31" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>